<commit_message>
Your message about the changes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAFI\Desktop\thesis\desco\phase 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAFI\Desktop\thesis\desco\phase 3\desco-predict-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACF186-9E52-4695-A3D4-4F65A4B35F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019516C0-92F3-40AF-8AA8-313AA395FD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CE84B220-09CC-4126-81F3-C4B37D047CE0}"/>
   </bookViews>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B74CC1F-6BC2-4A9B-829A-E9E0FD7631E7}">
   <dimension ref="A1:I791"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A756" workbookViewId="0">
+      <selection activeCell="J795" sqref="I764:J795"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23048,816 +23048,88 @@
       </c>
     </row>
     <row r="764" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A764" s="1">
-        <v>45689</v>
-      </c>
-      <c r="B764">
-        <v>23</v>
-      </c>
-      <c r="C764">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="D764">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="E764">
-        <v>100</v>
-      </c>
-      <c r="F764">
-        <v>2.8</v>
-      </c>
-      <c r="G764">
-        <v>48.6</v>
-      </c>
-      <c r="H764">
-        <v>158.1</v>
-      </c>
-      <c r="I764">
-        <v>851.04</v>
-      </c>
+      <c r="A764" s="1"/>
     </row>
     <row r="765" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A765" s="1">
-        <v>45690</v>
-      </c>
-      <c r="B765">
-        <v>23.2</v>
-      </c>
-      <c r="C765">
-        <v>18.3</v>
-      </c>
-      <c r="D765">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="E765">
-        <v>0</v>
-      </c>
-      <c r="F765">
-        <v>4.2</v>
-      </c>
-      <c r="G765">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="H765">
-        <v>185.1</v>
-      </c>
-      <c r="I765">
-        <v>803.52</v>
-      </c>
+      <c r="A765" s="1"/>
     </row>
     <row r="766" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A766" s="1">
-        <v>45691</v>
-      </c>
-      <c r="B766">
-        <v>22.5</v>
-      </c>
-      <c r="C766">
-        <v>15</v>
-      </c>
-      <c r="D766">
-        <v>67.7</v>
-      </c>
-      <c r="E766">
-        <v>0</v>
-      </c>
-      <c r="F766">
-        <v>3.6</v>
-      </c>
-      <c r="G766">
-        <v>31.2</v>
-      </c>
-      <c r="H766">
-        <v>205.6</v>
-      </c>
-      <c r="I766">
-        <v>884.23</v>
-      </c>
+      <c r="A766" s="1"/>
     </row>
     <row r="767" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A767" s="1">
-        <v>45692</v>
-      </c>
-      <c r="B767">
-        <v>21.5</v>
-      </c>
-      <c r="C767">
-        <v>12.9</v>
-      </c>
-      <c r="D767">
-        <v>60</v>
-      </c>
-      <c r="E767">
-        <v>0</v>
-      </c>
-      <c r="F767">
-        <v>6</v>
-      </c>
-      <c r="G767">
-        <v>5.3</v>
-      </c>
-      <c r="H767">
-        <v>214.4</v>
-      </c>
-      <c r="I767">
-        <v>839.31</v>
-      </c>
+      <c r="A767" s="1"/>
     </row>
     <row r="768" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A768" s="1">
-        <v>45693</v>
-      </c>
-      <c r="B768">
-        <v>22.5</v>
-      </c>
-      <c r="C768">
-        <v>15.2</v>
-      </c>
-      <c r="D768">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="E768">
-        <v>0</v>
-      </c>
-      <c r="F768">
-        <v>2.6</v>
-      </c>
-      <c r="G768">
-        <v>23.2</v>
-      </c>
-      <c r="H768">
-        <v>209.5</v>
-      </c>
-      <c r="I768">
-        <v>859.26</v>
-      </c>
-    </row>
-    <row r="769" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A769" s="1">
-        <v>45694</v>
-      </c>
-      <c r="B769">
-        <v>23.2</v>
-      </c>
-      <c r="C769">
-        <v>14.5</v>
-      </c>
-      <c r="D769">
-        <v>61.5</v>
-      </c>
-      <c r="E769">
-        <v>0</v>
-      </c>
-      <c r="F769">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G769">
-        <v>13.5</v>
-      </c>
-      <c r="H769">
-        <v>212.5</v>
-      </c>
-      <c r="I769">
-        <v>895.47</v>
-      </c>
-    </row>
-    <row r="770" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A770" s="1">
-        <v>45695</v>
-      </c>
-      <c r="B770">
-        <v>21.2</v>
-      </c>
-      <c r="C770">
-        <v>8.1</v>
-      </c>
-      <c r="D770">
-        <v>45.1</v>
-      </c>
-      <c r="E770">
-        <v>0</v>
-      </c>
-      <c r="F770">
-        <v>7.1</v>
-      </c>
-      <c r="G770">
-        <v>0</v>
-      </c>
-      <c r="H770">
-        <v>229.2</v>
-      </c>
-      <c r="I770">
-        <v>771.11</v>
-      </c>
-    </row>
-    <row r="771" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A771" s="1">
-        <v>45696</v>
-      </c>
-      <c r="B771">
-        <v>20.7</v>
-      </c>
-      <c r="C771">
-        <v>6.9</v>
-      </c>
-      <c r="D771">
-        <v>44.4</v>
-      </c>
-      <c r="E771">
-        <v>0</v>
-      </c>
-      <c r="F771">
-        <v>6.9</v>
-      </c>
-      <c r="G771">
-        <v>6.7</v>
-      </c>
-      <c r="H771">
-        <v>229.4</v>
-      </c>
-      <c r="I771">
-        <v>801.47</v>
-      </c>
-    </row>
-    <row r="772" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A772" s="1">
-        <v>45697</v>
-      </c>
-      <c r="B772">
-        <v>20.5</v>
-      </c>
-      <c r="C772">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D772">
-        <v>49.7</v>
-      </c>
-      <c r="E772">
-        <v>0</v>
-      </c>
-      <c r="F772">
-        <v>5.6</v>
-      </c>
-      <c r="G772">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H772">
-        <v>226.4</v>
-      </c>
-      <c r="I772">
-        <v>823.93</v>
-      </c>
-    </row>
-    <row r="773" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A773" s="1">
-        <v>45698</v>
-      </c>
-      <c r="B773">
-        <v>21.2</v>
-      </c>
-      <c r="C773">
-        <v>11.3</v>
-      </c>
-      <c r="D773">
-        <v>57.5</v>
-      </c>
-      <c r="E773">
-        <v>0</v>
-      </c>
-      <c r="F773">
-        <v>2.7</v>
-      </c>
-      <c r="G773">
-        <v>17.2</v>
-      </c>
-      <c r="H773">
-        <v>225.6</v>
-      </c>
-      <c r="I773">
-        <v>841.05</v>
-      </c>
-    </row>
-    <row r="774" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A774" s="1">
-        <v>45699</v>
-      </c>
-      <c r="B774">
-        <v>22.6</v>
-      </c>
-      <c r="C774">
-        <v>15.9</v>
-      </c>
-      <c r="D774">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="E774">
-        <v>100</v>
-      </c>
-      <c r="F774">
-        <v>4.7</v>
-      </c>
-      <c r="G774">
-        <v>28.2</v>
-      </c>
-      <c r="H774">
-        <v>205.3</v>
-      </c>
-      <c r="I774">
-        <v>893.79</v>
-      </c>
-    </row>
-    <row r="775" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A775" s="1">
-        <v>45700</v>
-      </c>
-      <c r="B775">
-        <v>23.8</v>
-      </c>
-      <c r="C775">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="D775">
-        <v>75.5</v>
-      </c>
-      <c r="E775">
-        <v>100</v>
-      </c>
-      <c r="F775">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G775">
-        <v>44.6</v>
-      </c>
-      <c r="H775">
-        <v>189.4</v>
-      </c>
-      <c r="I775">
-        <v>911.83</v>
-      </c>
-    </row>
-    <row r="776" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A776" s="1">
-        <v>45701</v>
-      </c>
-      <c r="B776">
-        <v>25.1</v>
-      </c>
-      <c r="C776">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="D776">
-        <v>70</v>
-      </c>
-      <c r="E776">
-        <v>0</v>
-      </c>
-      <c r="F776">
-        <v>5.9</v>
-      </c>
-      <c r="G776">
-        <v>28.2</v>
-      </c>
-      <c r="H776">
-        <v>161</v>
-      </c>
-      <c r="I776">
-        <v>935.14</v>
-      </c>
-    </row>
-    <row r="777" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A777" s="1">
-        <v>45702</v>
-      </c>
-      <c r="B777">
-        <v>22.6</v>
-      </c>
-      <c r="C777">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="D777">
-        <v>48.3</v>
-      </c>
-      <c r="E777">
-        <v>0</v>
-      </c>
-      <c r="F777">
-        <v>7.3</v>
-      </c>
-      <c r="G777">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H777">
-        <v>238.2</v>
-      </c>
-      <c r="I777">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="778" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A778" s="1">
-        <v>45703</v>
-      </c>
-      <c r="B778">
-        <v>22.3</v>
-      </c>
-      <c r="C778">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D778">
-        <v>44.7</v>
-      </c>
-      <c r="E778">
-        <v>0</v>
-      </c>
-      <c r="F778">
-        <v>4.3</v>
-      </c>
-      <c r="G778">
-        <v>11.9</v>
-      </c>
-      <c r="H778">
-        <v>233.8</v>
-      </c>
-      <c r="I778">
-        <v>699.25</v>
-      </c>
-    </row>
-    <row r="779" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A779" s="1">
-        <v>45704</v>
-      </c>
-      <c r="B779">
-        <v>23.2</v>
-      </c>
-      <c r="C779">
-        <v>12.5</v>
-      </c>
-      <c r="D779">
-        <v>55</v>
-      </c>
-      <c r="E779">
-        <v>0</v>
-      </c>
-      <c r="F779">
-        <v>3.9</v>
-      </c>
-      <c r="G779">
-        <v>6.1</v>
-      </c>
-      <c r="H779">
-        <v>230.4</v>
-      </c>
-      <c r="I779">
-        <v>850.42</v>
-      </c>
-    </row>
-    <row r="780" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A780" s="1">
-        <v>45705</v>
-      </c>
-      <c r="B780">
-        <v>24.4</v>
-      </c>
-      <c r="C780">
-        <v>17</v>
-      </c>
-      <c r="D780">
-        <v>66.099999999999994</v>
-      </c>
-      <c r="E780">
-        <v>100</v>
-      </c>
-      <c r="F780">
-        <v>3.7</v>
-      </c>
-      <c r="G780">
-        <v>27.2</v>
-      </c>
-      <c r="H780">
-        <v>218.6</v>
-      </c>
-      <c r="I780">
-        <v>915.59</v>
-      </c>
-    </row>
-    <row r="781" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A781" s="1">
-        <v>45706</v>
-      </c>
-      <c r="B781">
-        <v>25</v>
-      </c>
-      <c r="C781">
-        <v>19.3</v>
-      </c>
-      <c r="D781">
-        <v>71.8</v>
-      </c>
-      <c r="E781">
-        <v>100</v>
-      </c>
-      <c r="F781">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G781">
-        <v>26.5</v>
-      </c>
-      <c r="H781">
-        <v>217.4</v>
-      </c>
-      <c r="I781">
-        <v>978.86</v>
-      </c>
-    </row>
-    <row r="782" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A782" s="1">
-        <v>45707</v>
-      </c>
-      <c r="B782">
-        <v>25.1</v>
-      </c>
-      <c r="C782">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="D782">
-        <v>59.9</v>
-      </c>
-      <c r="E782">
-        <v>100</v>
-      </c>
-      <c r="F782">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G782">
-        <v>29.7</v>
-      </c>
-      <c r="H782">
-        <v>196.8</v>
-      </c>
-      <c r="I782">
-        <v>955.5</v>
-      </c>
-    </row>
-    <row r="783" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A783" s="1">
-        <v>45708</v>
-      </c>
-      <c r="B783">
-        <v>24.9</v>
-      </c>
-      <c r="C783">
-        <v>15.8</v>
-      </c>
-      <c r="D783">
-        <v>60.8</v>
-      </c>
-      <c r="E783">
-        <v>100</v>
-      </c>
-      <c r="F783">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G783">
-        <v>44.9</v>
-      </c>
-      <c r="H783">
-        <v>212.5</v>
-      </c>
-      <c r="I783">
-        <v>965.95</v>
-      </c>
-    </row>
-    <row r="784" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A784" s="1">
-        <v>45709</v>
-      </c>
-      <c r="B784">
-        <v>25.2</v>
-      </c>
-      <c r="C784">
-        <v>16.8</v>
-      </c>
-      <c r="D784">
-        <v>62.9</v>
-      </c>
-      <c r="E784">
-        <v>0</v>
-      </c>
-      <c r="F784">
-        <v>4.8</v>
-      </c>
-      <c r="G784">
-        <v>22.2</v>
-      </c>
-      <c r="H784">
-        <v>220.4</v>
-      </c>
-      <c r="I784">
-        <v>801.04</v>
-      </c>
-    </row>
-    <row r="785" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A785" s="1">
-        <v>45710</v>
-      </c>
-      <c r="B785">
-        <v>23.8</v>
-      </c>
-      <c r="C785">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D785">
-        <v>69.8</v>
-      </c>
-      <c r="E785">
-        <v>100</v>
-      </c>
-      <c r="F785">
-        <v>4.7</v>
-      </c>
-      <c r="G785">
-        <v>48.7</v>
-      </c>
-      <c r="H785">
-        <v>214</v>
-      </c>
-      <c r="I785">
-        <v>934.24</v>
-      </c>
-    </row>
-    <row r="786" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A786" s="1">
-        <v>45711</v>
-      </c>
-      <c r="B786">
-        <v>23.2</v>
-      </c>
-      <c r="C786">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="D786">
-        <v>67.3</v>
-      </c>
-      <c r="E786">
-        <v>100</v>
-      </c>
-      <c r="F786">
-        <v>5.9</v>
-      </c>
-      <c r="G786">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="H786">
-        <v>196.5</v>
-      </c>
-      <c r="I786">
-        <v>942.46</v>
-      </c>
-    </row>
-    <row r="787" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A787" s="1">
-        <v>45712</v>
-      </c>
-      <c r="B787">
-        <v>24</v>
-      </c>
-      <c r="C787">
-        <v>13.5</v>
-      </c>
-      <c r="D787">
-        <v>56.2</v>
-      </c>
-      <c r="E787">
-        <v>0</v>
-      </c>
-      <c r="F787">
-        <v>6.5</v>
-      </c>
-      <c r="G787">
-        <v>23.1</v>
-      </c>
-      <c r="H787">
-        <v>229.6</v>
-      </c>
-      <c r="I787">
-        <v>925.38</v>
-      </c>
-    </row>
-    <row r="788" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A788" s="1">
-        <v>45713</v>
-      </c>
-      <c r="B788">
-        <v>24.8</v>
-      </c>
-      <c r="C788">
-        <v>13.3</v>
-      </c>
-      <c r="D788">
-        <v>52</v>
-      </c>
-      <c r="E788">
-        <v>0</v>
-      </c>
-      <c r="F788">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G788">
-        <v>51</v>
-      </c>
-      <c r="H788">
-        <v>197</v>
-      </c>
-      <c r="I788">
-        <v>940.41</v>
-      </c>
-    </row>
-    <row r="789" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A789" s="1">
-        <v>45714</v>
-      </c>
-      <c r="B789">
-        <v>24.3</v>
-      </c>
-      <c r="C789">
-        <v>10.8</v>
-      </c>
-      <c r="D789">
-        <v>48</v>
-      </c>
-      <c r="E789">
-        <v>0</v>
-      </c>
-      <c r="F789">
-        <v>10.3</v>
-      </c>
-      <c r="G789">
-        <v>28.4</v>
-      </c>
-      <c r="H789">
-        <v>252.5</v>
-      </c>
-      <c r="I789">
-        <v>944.02</v>
-      </c>
-    </row>
-    <row r="790" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A790" s="1">
-        <v>45715</v>
-      </c>
-      <c r="B790">
-        <v>24.5</v>
-      </c>
-      <c r="C790">
-        <v>12.7</v>
-      </c>
-      <c r="D790">
-        <v>50.2</v>
-      </c>
-      <c r="E790">
-        <v>0</v>
-      </c>
-      <c r="F790">
-        <v>6.4</v>
-      </c>
-      <c r="G790">
-        <v>19.3</v>
-      </c>
-      <c r="H790">
-        <v>246.4</v>
-      </c>
-      <c r="I790">
-        <v>949.68</v>
-      </c>
-    </row>
-    <row r="791" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A791" s="1">
-        <v>45716</v>
-      </c>
-      <c r="B791">
-        <v>25.1</v>
-      </c>
-      <c r="C791">
-        <v>15.6</v>
-      </c>
-      <c r="D791">
-        <v>57.2</v>
-      </c>
-      <c r="E791">
-        <v>0</v>
-      </c>
-      <c r="F791">
-        <v>2.8</v>
-      </c>
-      <c r="G791">
-        <v>32.6</v>
-      </c>
-      <c r="H791">
-        <v>202.3</v>
-      </c>
-      <c r="I791">
-        <v>882.81</v>
-      </c>
+      <c r="A768" s="1"/>
+    </row>
+    <row r="769" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A769" s="1"/>
+    </row>
+    <row r="770" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A770" s="1"/>
+    </row>
+    <row r="771" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A771" s="1"/>
+    </row>
+    <row r="772" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A772" s="1"/>
+    </row>
+    <row r="773" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A773" s="1"/>
+    </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A774" s="1"/>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A775" s="1"/>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A776" s="1"/>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A777" s="1"/>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A778" s="1"/>
+    </row>
+    <row r="779" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A779" s="1"/>
+    </row>
+    <row r="780" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A780" s="1"/>
+    </row>
+    <row r="781" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A781" s="1"/>
+    </row>
+    <row r="782" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A782" s="1"/>
+    </row>
+    <row r="783" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A783" s="1"/>
+    </row>
+    <row r="784" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A784" s="1"/>
+    </row>
+    <row r="785" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A785" s="1"/>
+    </row>
+    <row r="786" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A786" s="1"/>
+    </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A787" s="1"/>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A788" s="1"/>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A789" s="1"/>
+    </row>
+    <row r="790" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A790" s="1"/>
+    </row>
+    <row r="791" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A791" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>